<commit_message>
Added bar codes, serial numbers, recovery dates where needed
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_CP02PMUI_00001.xlsx
+++ b/deployment/Omaha_Cal_Info_CP02PMUI_00001.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AST1799\Documents\OOI\OOI Douments\CI\asset-management\deployment\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6795" yWindow="6285" windowWidth="20730" windowHeight="11760" tabRatio="377" activeTab="1"/>
+    <workbookView xWindow="6795" yWindow="6285" windowWidth="20730" windowHeight="11760" tabRatio="377"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="1" r:id="rId1"/>
@@ -30,7 +35,7 @@
     <definedName name="_FilterDatabase_1_1_1">Moorings!$B$1:$K$80</definedName>
     <definedName name="_FilterDatabase_2">Asset_Cal_Info!$A$1:$H$403</definedName>
   </definedNames>
-  <calcPr calcId="140001"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -40,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="85">
   <si>
     <t>Ref Des</t>
   </si>
@@ -332,6 +337,15 @@
   <si>
     <t>43-2497</t>
   </si>
+  <si>
+    <t>CP02PMUI-WFP01-01-VEL3DK000</t>
+  </si>
+  <si>
+    <t>OL000331</t>
+  </si>
+  <si>
+    <t>OL000332</t>
+  </si>
 </sst>
 </file>
 
@@ -340,7 +354,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -369,12 +383,6 @@
       <name val="DejaVu Sans Mono"/>
       <family val="3"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -514,15 +522,15 @@
   </borders>
   <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -542,48 +550,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -722,7 +730,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -757,7 +765,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -968,8 +976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -988,40 +996,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="25.5">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="23" t="s">
+      <c r="C1" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="I1" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="23" t="s">
+      <c r="J1" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="K1" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="23" t="s">
+      <c r="L1" s="22" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1060,8 +1068,14 @@
         <v>42</v>
       </c>
       <c r="L2" s="4"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
+      <c r="M2" s="23">
+        <f>((LEFT(H2,(FIND("°",H2,1)-1)))+(MID(H2,(FIND("°",H2,1)+1),(FIND("'",H2,1))-(FIND("°",H2,1)+1))/60))*(IF(RIGHT(H2,1)="N",1,-1))</f>
+        <v>40.363405</v>
+      </c>
+      <c r="N2" s="23">
+        <f>((LEFT(I2,(FIND("°",I2,1)-1)))+(MID(I2,(FIND("°",I2,1)+1),(FIND("'",I2,1))-(FIND("°",I2,1)+1))/60))*(IF(RIGHT(I2,1)="E",1,-1))</f>
+        <v>-70.775988333333331</v>
+      </c>
     </row>
     <row r="3" spans="1:14">
       <c r="E3" s="6"/>
@@ -1084,10 +1098,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:P40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="A10" sqref="A1:A1048576"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1103,7 +1117,7 @@
     <col min="9" max="9" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="31.5">
+    <row r="1" spans="1:16" ht="31.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1129,145 +1143,213 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="14" t="s">
+    <row r="2" spans="1:16">
+      <c r="A2" s="13" t="s">
         <v>69</v>
       </c>
       <c r="B2" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2" s="15">
+      <c r="C2" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="14">
         <v>1</v>
       </c>
       <c r="E2" t="s">
         <v>80</v>
       </c>
-      <c r="F2" s="15">
+      <c r="F2" s="14">
         <v>19336</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="16">
+      <c r="H2" s="15">
         <v>73000</v>
       </c>
-      <c r="I2" s="22" t="s">
+      <c r="I2" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="J2" s="14"/>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="14" t="s">
+      <c r="J2" s="13"/>
+      <c r="K2">
+        <f>MATCH(A2,L:L,0)</f>
+        <v>4</v>
+      </c>
+      <c r="L2" t="s">
+        <v>60</v>
+      </c>
+      <c r="P2">
+        <f>MATCH(L2,A:A,0)</f>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" s="13" t="s">
         <v>69</v>
       </c>
       <c r="B3" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D3" s="15">
+      <c r="C3" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="14">
         <v>1</v>
       </c>
       <c r="E3" t="s">
         <v>80</v>
       </c>
-      <c r="F3" s="15">
+      <c r="F3" s="14">
         <v>19336</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="16">
+      <c r="H3" s="15">
         <v>40.363405</v>
       </c>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="14" t="s">
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3">
+        <f t="shared" ref="K3:K39" si="0">MATCH(A3,L:L,0)</f>
+        <v>4</v>
+      </c>
+      <c r="L3" t="s">
+        <v>38</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P10" si="1">MATCH(L3,A:A,0)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" s="13" t="s">
         <v>69</v>
       </c>
       <c r="B4" t="s">
         <v>72</v>
       </c>
-      <c r="C4" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" s="15">
+      <c r="C4" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="14">
         <v>1</v>
       </c>
       <c r="E4" t="s">
         <v>80</v>
       </c>
-      <c r="F4" s="15">
+      <c r="F4" s="14">
         <v>19336</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="16">
+      <c r="H4" s="15">
         <v>-70.775988333333331</v>
       </c>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="14" t="s">
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="L4" t="s">
+        <v>69</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" s="13"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="L5" t="s">
+        <v>59</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" s="13" t="s">
         <v>38</v>
       </c>
       <c r="B6" t="s">
         <v>72</v>
       </c>
-      <c r="C6" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D6" s="15">
-        <v>1</v>
-      </c>
-      <c r="E6" s="15"/>
-      <c r="F6" s="20" t="s">
+      <c r="C6" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="14">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>83</v>
+      </c>
+      <c r="F6" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="G6" s="14"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="21" t="s">
+      <c r="G6" s="13"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="J6" s="14"/>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="J6" s="13"/>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="L6" t="s">
+        <v>82</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
-      <c r="F7" s="12"/>
-      <c r="H7" s="13"/>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="14" t="s">
+      <c r="F7" s="11"/>
+      <c r="H7" s="12"/>
+      <c r="K7" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="L7" t="s">
         <v>18</v>
       </c>
+      <c r="P7">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" s="13" t="s">
+        <v>18</v>
+      </c>
       <c r="B8" t="s">
         <v>72</v>
       </c>
-      <c r="C8" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" s="15">
+      <c r="C8" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="14">
         <v>1</v>
       </c>
       <c r="E8" t="s">
@@ -1276,28 +1358,39 @@
       <c r="F8" t="s">
         <v>81</v>
       </c>
-      <c r="G8" s="14" t="s">
+      <c r="G8" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="17">
+      <c r="H8" s="16">
         <v>-837.37</v>
       </c>
       <c r="I8" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="J8" s="14"/>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="14" t="s">
+      <c r="J8" s="13"/>
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="L8" t="s">
+        <v>25</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" s="13" t="s">
         <v>18</v>
       </c>
       <c r="B9" t="s">
         <v>72</v>
       </c>
-      <c r="C9" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D9" s="15">
+      <c r="C9" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="14">
         <v>1</v>
       </c>
       <c r="E9" t="s">
@@ -1306,26 +1399,37 @@
       <c r="F9" t="s">
         <v>81</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="G9" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="16">
+      <c r="H9" s="15">
         <v>40.363405</v>
       </c>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="14" t="s">
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="L9" t="s">
+        <v>28</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" s="13" t="s">
         <v>18</v>
       </c>
       <c r="B10" t="s">
         <v>72</v>
       </c>
-      <c r="C10" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D10" s="15">
+      <c r="C10" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="14">
         <v>1</v>
       </c>
       <c r="E10" t="s">
@@ -1334,26 +1438,37 @@
       <c r="F10" t="s">
         <v>81</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="G10" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="H10" s="16">
+      <c r="H10" s="15">
         <v>-70.775988333333331</v>
       </c>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="14" t="s">
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="L10" t="s">
+        <v>35</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" s="13" t="s">
         <v>18</v>
       </c>
       <c r="B11" t="s">
         <v>72</v>
       </c>
-      <c r="C11" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" s="15">
+      <c r="C11" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="14">
         <v>1</v>
       </c>
       <c r="E11" t="s">
@@ -1362,28 +1477,32 @@
       <c r="F11" t="s">
         <v>81</v>
       </c>
-      <c r="G11" s="14" t="s">
+      <c r="G11" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="H11" s="17">
+      <c r="H11" s="16">
         <v>2.5849999999999999E-4</v>
       </c>
       <c r="I11" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="J11" s="14"/>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="14" t="s">
+      <c r="J11" s="13"/>
+      <c r="K11">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" s="13" t="s">
         <v>18</v>
       </c>
       <c r="B12" t="s">
         <v>72</v>
       </c>
-      <c r="C12" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="15">
+      <c r="C12" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="14">
         <v>1</v>
       </c>
       <c r="E12" t="s">
@@ -1392,28 +1511,32 @@
       <c r="F12" t="s">
         <v>81</v>
       </c>
-      <c r="G12" s="14" t="s">
+      <c r="G12" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="H12" s="17">
+      <c r="H12" s="16">
         <v>-3.3024999999999999E-3</v>
       </c>
       <c r="I12" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="J12" s="14"/>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="14" t="s">
+      <c r="J12" s="13"/>
+      <c r="K12">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" s="13" t="s">
         <v>18</v>
       </c>
       <c r="B13" t="s">
         <v>72</v>
       </c>
-      <c r="C13" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="15">
+      <c r="C13" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="14">
         <v>1</v>
       </c>
       <c r="E13" t="s">
@@ -1422,28 +1545,32 @@
       <c r="F13" t="s">
         <v>81</v>
       </c>
-      <c r="G13" s="14" t="s">
+      <c r="G13" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="H13" s="17">
+      <c r="H13" s="16">
         <v>1.9880000000000001E-4</v>
       </c>
       <c r="I13" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="J13" s="14"/>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="14" t="s">
+      <c r="J13" s="13"/>
+      <c r="K13">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14" s="13" t="s">
         <v>18</v>
       </c>
       <c r="B14" t="s">
         <v>72</v>
       </c>
-      <c r="C14" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" s="15">
+      <c r="C14" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="14">
         <v>1</v>
       </c>
       <c r="E14" t="s">
@@ -1452,28 +1579,32 @@
       <c r="F14" t="s">
         <v>81</v>
       </c>
-      <c r="G14" s="14" t="s">
+      <c r="G14" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="H14" s="17">
+      <c r="H14" s="16">
         <v>-3.0292999999999999E-6</v>
       </c>
       <c r="I14" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="J14" s="14"/>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" s="14" t="s">
+      <c r="J14" s="13"/>
+      <c r="K14">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15" s="13" t="s">
         <v>18</v>
       </c>
       <c r="B15" t="s">
         <v>72</v>
       </c>
-      <c r="C15" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15" s="15">
+      <c r="C15" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="14">
         <v>1</v>
       </c>
       <c r="E15" t="s">
@@ -1482,560 +1613,648 @@
       <c r="F15" t="s">
         <v>81</v>
       </c>
-      <c r="G15" s="14" t="s">
+      <c r="G15" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="H15" s="17">
+      <c r="H15" s="16">
         <v>3.5999999999999997E-2</v>
       </c>
       <c r="I15" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="J15" s="14"/>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" s="14"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-    </row>
-    <row r="17" spans="1:10">
-      <c r="A17" s="14" t="s">
+      <c r="J15" s="13"/>
+      <c r="K15">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16" s="13"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="13" t="s">
         <v>25</v>
       </c>
       <c r="B17" t="s">
         <v>72</v>
       </c>
-      <c r="C17" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" s="15">
+      <c r="C17" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="14">
         <v>1</v>
       </c>
       <c r="E17" t="s">
         <v>78</v>
       </c>
-      <c r="F17" s="15">
+      <c r="F17" s="14">
         <v>111</v>
       </c>
-      <c r="G17" s="14" t="s">
+      <c r="G17" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H17" s="16">
+      <c r="H17" s="15">
         <v>40.363405</v>
       </c>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="A18" s="14" t="s">
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="13" t="s">
         <v>25</v>
       </c>
       <c r="B18" t="s">
         <v>72</v>
       </c>
-      <c r="C18" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D18" s="15">
+      <c r="C18" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="14">
         <v>1</v>
       </c>
       <c r="E18" t="s">
         <v>78</v>
       </c>
-      <c r="F18" s="15">
+      <c r="F18" s="14">
         <v>111</v>
       </c>
-      <c r="G18" s="14" t="s">
+      <c r="G18" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="H18" s="16">
+      <c r="H18" s="15">
         <v>-70.775988333333331</v>
       </c>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-    </row>
-    <row r="19" spans="1:10">
-      <c r="A19" s="14"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-    </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="14" t="s">
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="13"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" s="13" t="s">
         <v>67</v>
       </c>
       <c r="B20" t="s">
         <v>72</v>
       </c>
-      <c r="C20" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D20" s="15">
+      <c r="C20" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="14">
         <v>1</v>
       </c>
       <c r="E20" t="s">
         <v>77</v>
       </c>
-      <c r="F20" s="18">
+      <c r="F20" s="17">
         <v>100015</v>
       </c>
-      <c r="G20" s="14" t="s">
+      <c r="G20" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="H20" s="16">
+      <c r="H20" s="15">
         <v>40.363405</v>
       </c>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-    </row>
-    <row r="21" spans="1:10">
-      <c r="A21" s="14" t="s">
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="13" t="s">
         <v>67</v>
       </c>
       <c r="B21" t="s">
         <v>72</v>
       </c>
-      <c r="C21" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D21" s="15">
+      <c r="C21" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="14">
         <v>1</v>
       </c>
       <c r="E21" t="s">
         <v>77</v>
       </c>
-      <c r="F21" s="18">
+      <c r="F21" s="17">
         <v>100015</v>
       </c>
-      <c r="G21" s="14" t="s">
+      <c r="G21" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="H21" s="16">
+      <c r="H21" s="15">
         <v>-70.775988333333331</v>
       </c>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-    </row>
-    <row r="22" spans="1:10">
-      <c r="A22" s="14"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
-    </row>
-    <row r="23" spans="1:10">
-      <c r="A23" s="14" t="s">
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" s="13"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+      <c r="K22" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" s="13" t="s">
         <v>28</v>
       </c>
       <c r="B23" t="s">
         <v>72</v>
       </c>
-      <c r="C23" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D23" s="15">
+      <c r="C23" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="14">
         <v>1</v>
       </c>
       <c r="E23" t="s">
         <v>76</v>
       </c>
-      <c r="F23" s="15">
+      <c r="F23" s="14">
         <v>1029</v>
       </c>
-      <c r="G23" s="14" t="s">
+      <c r="G23" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="H23" s="16">
+      <c r="H23" s="15">
         <v>1.0760000000000001</v>
       </c>
-      <c r="I23" s="15" t="s">
+      <c r="I23" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="J23" s="14"/>
-    </row>
-    <row r="24" spans="1:10">
-      <c r="A24" s="14" t="s">
+      <c r="J23" s="13"/>
+      <c r="K23">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" s="13" t="s">
         <v>28</v>
       </c>
       <c r="B24" t="s">
         <v>72</v>
       </c>
-      <c r="C24" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D24" s="15">
+      <c r="C24" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" s="14">
         <v>1</v>
       </c>
       <c r="E24" t="s">
         <v>76</v>
       </c>
-      <c r="F24" s="15">
+      <c r="F24" s="14">
         <v>1029</v>
       </c>
-      <c r="G24" s="14" t="s">
+      <c r="G24" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="H24" s="16">
+      <c r="H24" s="15">
         <v>50</v>
       </c>
       <c r="I24" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="J24" s="14"/>
-    </row>
-    <row r="25" spans="1:10">
-      <c r="A25" s="14" t="s">
+      <c r="J24" s="13"/>
+      <c r="K24">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" s="13" t="s">
         <v>28</v>
       </c>
       <c r="B25" t="s">
         <v>72</v>
       </c>
-      <c r="C25" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D25" s="15">
+      <c r="C25" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" s="14">
         <v>1</v>
       </c>
       <c r="E25" t="s">
         <v>76</v>
       </c>
-      <c r="F25" s="15">
+      <c r="F25" s="14">
         <v>1029</v>
       </c>
-      <c r="G25" s="14" t="s">
+      <c r="G25" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="H25" s="16">
+      <c r="H25" s="15">
         <v>53</v>
       </c>
       <c r="I25" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="J25" s="14"/>
-    </row>
-    <row r="26" spans="1:10">
-      <c r="A26" s="14" t="s">
+      <c r="J25" s="13"/>
+      <c r="K25">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26" s="13" t="s">
         <v>28</v>
       </c>
       <c r="B26" t="s">
         <v>72</v>
       </c>
-      <c r="C26" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D26" s="15">
+      <c r="C26" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" s="14">
         <v>1</v>
       </c>
       <c r="E26" t="s">
         <v>76</v>
       </c>
-      <c r="F26" s="15">
+      <c r="F26" s="14">
         <v>1029</v>
       </c>
-      <c r="G26" s="14" t="s">
+      <c r="G26" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="H26" s="16">
+      <c r="H26" s="15">
         <v>50</v>
       </c>
       <c r="I26" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="J26" s="14"/>
-    </row>
-    <row r="27" spans="1:10">
-      <c r="A27" s="14" t="s">
+      <c r="J26" s="13"/>
+      <c r="K26">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27" s="13" t="s">
         <v>28</v>
       </c>
       <c r="B27" t="s">
         <v>72</v>
       </c>
-      <c r="C27" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D27" s="15">
+      <c r="C27" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27" s="14">
         <v>1</v>
       </c>
       <c r="E27" t="s">
         <v>76</v>
       </c>
-      <c r="F27" s="15">
+      <c r="F27" s="14">
         <v>1029</v>
       </c>
-      <c r="G27" s="14" t="s">
+      <c r="G27" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="H27" s="16">
+      <c r="H27" s="15">
         <v>3.9E-2</v>
       </c>
-      <c r="I27" s="15" t="s">
+      <c r="I27" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="J27" s="14"/>
-    </row>
-    <row r="28" spans="1:10">
-      <c r="A28" s="14" t="s">
+      <c r="J27" s="13"/>
+      <c r="K27">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28" s="13" t="s">
         <v>28</v>
       </c>
       <c r="B28" t="s">
         <v>72</v>
       </c>
-      <c r="C28" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D28" s="15">
+      <c r="C28" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28" s="14">
         <v>1</v>
       </c>
       <c r="E28" t="s">
         <v>76</v>
       </c>
-      <c r="F28" s="15">
+      <c r="F28" s="14">
         <v>1029</v>
       </c>
-      <c r="G28" s="14" t="s">
+      <c r="G28" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="H28" s="16">
+      <c r="H28" s="15">
         <v>700</v>
       </c>
-      <c r="I28" s="15" t="s">
+      <c r="I28" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="J28" s="14"/>
-    </row>
-    <row r="29" spans="1:10">
-      <c r="A29" s="14" t="s">
+      <c r="J28" s="13"/>
+      <c r="K28">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29" s="13" t="s">
         <v>28</v>
       </c>
       <c r="B29" t="s">
         <v>72</v>
       </c>
-      <c r="C29" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D29" s="15">
+      <c r="C29" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D29" s="14">
         <v>1</v>
       </c>
       <c r="E29" t="s">
         <v>76</v>
       </c>
-      <c r="F29" s="15">
+      <c r="F29" s="14">
         <v>1029</v>
       </c>
-      <c r="G29" s="14" t="s">
+      <c r="G29" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="H29" s="16">
+      <c r="H29" s="15">
         <v>9.0700000000000003E-2</v>
       </c>
       <c r="I29" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="J29" s="14"/>
-    </row>
-    <row r="30" spans="1:10">
-      <c r="A30" s="14" t="s">
+      <c r="J29" s="13"/>
+      <c r="K29">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30" s="13" t="s">
         <v>28</v>
       </c>
       <c r="B30" t="s">
         <v>72</v>
       </c>
-      <c r="C30" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D30" s="15">
+      <c r="C30" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30" s="14">
         <v>1</v>
       </c>
       <c r="E30" t="s">
         <v>76</v>
       </c>
-      <c r="F30" s="15">
+      <c r="F30" s="14">
         <v>1029</v>
       </c>
-      <c r="G30" s="14" t="s">
+      <c r="G30" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="H30" s="16">
+      <c r="H30" s="15">
         <v>1.21E-2</v>
       </c>
       <c r="I30" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="J30" s="14"/>
-    </row>
-    <row r="31" spans="1:10">
-      <c r="A31" s="14" t="s">
+      <c r="J30" s="13"/>
+      <c r="K30">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31" s="13" t="s">
         <v>28</v>
       </c>
       <c r="B31" t="s">
         <v>72</v>
       </c>
-      <c r="C31" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D31" s="15">
+      <c r="C31" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D31" s="14">
         <v>1</v>
       </c>
       <c r="E31" t="s">
         <v>76</v>
       </c>
-      <c r="F31" s="15">
+      <c r="F31" s="14">
         <v>1029</v>
       </c>
-      <c r="G31" s="14" t="s">
+      <c r="G31" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="H31" s="19">
+      <c r="H31" s="18">
         <v>3.49E-6</v>
       </c>
       <c r="I31" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="J31" s="14"/>
-    </row>
-    <row r="32" spans="1:10">
-      <c r="A32" s="14" t="s">
+      <c r="J31" s="13"/>
+      <c r="K31">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="A32" s="13" t="s">
         <v>28</v>
       </c>
       <c r="B32" t="s">
         <v>72</v>
       </c>
-      <c r="C32" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D32" s="15">
+      <c r="C32" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D32" s="14">
         <v>1</v>
       </c>
       <c r="E32" t="s">
         <v>76</v>
       </c>
-      <c r="F32" s="15">
+      <c r="F32" s="14">
         <v>1029</v>
       </c>
-      <c r="G32" s="14" t="s">
+      <c r="G32" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="H32" s="16">
+      <c r="H32" s="15">
         <v>124</v>
       </c>
-      <c r="I32" s="15" t="s">
+      <c r="I32" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="J32" s="14"/>
-    </row>
-    <row r="33" spans="1:10">
-      <c r="A33" s="14"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="16"/>
-      <c r="I33" s="14"/>
-      <c r="J33" s="14"/>
-    </row>
-    <row r="34" spans="1:10">
-      <c r="A34" s="14" t="s">
+      <c r="J32" s="13"/>
+      <c r="K32">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="A33" s="13"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="13"/>
+      <c r="K33" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34" s="13" t="s">
         <v>35</v>
       </c>
       <c r="B34" t="s">
         <v>72</v>
       </c>
-      <c r="C34" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D34" s="15">
+      <c r="C34" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D34" s="14">
         <v>1</v>
       </c>
       <c r="E34" t="s">
         <v>75</v>
       </c>
-      <c r="F34" s="15">
+      <c r="F34" s="14">
         <v>20437</v>
       </c>
-      <c r="G34" s="14" t="s">
+      <c r="G34" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="H34" s="16">
+      <c r="H34" s="15">
         <v>1.5</v>
       </c>
       <c r="I34" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="J34" s="14"/>
-    </row>
-    <row r="35" spans="1:10">
-      <c r="A35" s="14" t="s">
+      <c r="J34" s="13"/>
+      <c r="K34">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="A35" s="13" t="s">
         <v>35</v>
       </c>
       <c r="B35" t="s">
         <v>72</v>
       </c>
-      <c r="C35" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D35" s="15">
+      <c r="C35" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D35" s="14">
         <v>1</v>
       </c>
       <c r="E35" t="s">
         <v>75</v>
       </c>
-      <c r="F35" s="15">
+      <c r="F35" s="14">
         <v>20437</v>
       </c>
-      <c r="G35" s="14" t="s">
+      <c r="G35" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="H35" s="19">
+      <c r="H35" s="18">
         <v>1.01E-17</v>
       </c>
       <c r="I35" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="J35" s="14"/>
-    </row>
-    <row r="36" spans="1:10">
-      <c r="A36" s="14"/>
-      <c r="B36" s="14"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="14"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="16"/>
-      <c r="I36" s="14"/>
-      <c r="J36" s="14"/>
-    </row>
-    <row r="37" spans="1:10">
-      <c r="A37" s="14" t="s">
+      <c r="J35" s="13"/>
+      <c r="K35">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
+      <c r="A36" s="13"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="13"/>
+      <c r="K36" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="A37" s="13" t="s">
         <v>59</v>
       </c>
       <c r="B37" t="s">
         <v>72</v>
       </c>
-      <c r="C37" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D37" s="15">
+      <c r="C37" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D37" s="14">
         <v>1</v>
       </c>
       <c r="E37" t="s">
@@ -2044,46 +2263,62 @@
       <c r="F37" t="s">
         <v>73</v>
       </c>
-      <c r="G37" s="14"/>
-      <c r="H37" s="16"/>
-      <c r="I37" s="14"/>
-      <c r="J37" s="14"/>
-    </row>
-    <row r="39" spans="1:10">
-      <c r="A39" s="14" t="s">
+      <c r="G37" s="13"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="13"/>
+      <c r="K37">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="K38" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
+      <c r="A39" s="13" t="s">
         <v>60</v>
       </c>
       <c r="B39" t="s">
         <v>72</v>
       </c>
-      <c r="C39" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D39" s="15">
-        <v>1</v>
-      </c>
-      <c r="E39" s="15"/>
-      <c r="F39" s="20" t="s">
+      <c r="C39" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D39" s="14">
+        <v>1</v>
+      </c>
+      <c r="E39" t="s">
+        <v>84</v>
+      </c>
+      <c r="F39" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="G39" s="14"/>
-      <c r="H39" s="16"/>
-      <c r="I39" s="21" t="s">
+      <c r="G39" s="13"/>
+      <c r="H39" s="15"/>
+      <c r="I39" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="J39" s="14"/>
-    </row>
-    <row r="40" spans="1:10">
-      <c r="A40" s="14"/>
-      <c r="B40" s="14"/>
-      <c r="C40" s="15"/>
-      <c r="D40" s="15"/>
-      <c r="E40" s="15"/>
-      <c r="F40" s="15"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="16"/>
-      <c r="I40" s="21"/>
-      <c r="J40" s="14"/>
+      <c r="J39" s="13"/>
+      <c r="K39">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
+      <c r="A40" s="13"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="15"/>
+      <c r="I40" s="20"/>
+      <c r="J40" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>